<commit_message>
Update Segmentation Mask label
</commit_message>
<xml_diff>
--- a/segmentation-mask/latest/segmentation-mask.xlsx
+++ b/segmentation-mask/latest/segmentation-mask.xlsx
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>parent_dataset_id</t>
   </si>
@@ -118,7 +118,7 @@
     <t>derived_dataset_type</t>
   </si>
   <si>
-    <t>Segmentation mask</t>
+    <t>Segmentation Mask</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000314</t>
@@ -151,9 +151,6 @@
     <t>schema:title</t>
   </si>
   <si>
-    <t>Segmentation Mask</t>
-  </si>
-  <si>
     <t>pav:version</t>
   </si>
   <si>
@@ -163,7 +160,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-08-05T13:25:47-07:00</t>
+    <t>2024-08-07T09:56:44-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -376,27 +373,27 @@
         <v>14</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>